<commit_message>
Inserido tratamento de download fora do prazo do roteiro.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Roteiros.xlsx
+++ b/leda-submission-server/conf/Roteiros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Roteiro</t>
   </si>
@@ -43,37 +43,40 @@
     <t>Roteiro de revisao de Junit e recursao</t>
   </si>
   <si>
-    <t>R01</t>
+    <t>R01-01</t>
   </si>
   <si>
-    <t>Ordenacao por comparacao iterativa</t>
+    <t>Ordenacao por comparacao iterativa, bubble bidirecional</t>
   </si>
   <si>
-    <t>R02</t>
+    <t>R01-02</t>
+  </si>
+  <si>
+    <t>Ordenacao por comparacao iterativa, selection bidirecional</t>
+  </si>
+  <si>
+    <t>R02-01</t>
   </si>
   <si>
     <t>Ordenacao por comparacao recursivo</t>
   </si>
   <si>
-    <t>R03</t>
+    <t>R02-02</t>
+  </si>
+  <si>
+    <t>R03-01</t>
   </si>
   <si>
     <t>Ordenacao linear</t>
+  </si>
+  <si>
+    <t>R03-02</t>
   </si>
   <si>
     <t>R04</t>
   </si>
   <si>
     <t>R05</t>
-  </si>
-  <si>
-    <t>R06</t>
-  </si>
-  <si>
-    <t>R07</t>
-  </si>
-  <si>
-    <t>R08</t>
   </si>
   <si>
     <t>R09</t>
@@ -199,7 +202,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="7.63"/>
-    <col customWidth="1" min="2" max="2" width="31.38"/>
+    <col customWidth="1" min="2" max="2" width="50.25"/>
     <col customWidth="1" min="3" max="3" width="17.13"/>
     <col customWidth="1" min="4" max="4" width="22.88"/>
     <col customWidth="1" min="5" max="5" width="20.13"/>
@@ -264,7 +267,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -292,7 +295,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -320,7 +323,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -348,36 +351,40 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C6" s="4">
-        <v>42564.666666666664</v>
+        <v>42562.583333333336</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>14/07/2016 04:00:00</v>
+        <v>12/07/2016 02:00:00</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>15/07/2016 16:00:00</v>
+        <v>13/07/2016 14:00:00</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>16/07/2016 16:00:00</v>
+        <v>14/07/2016 14:00:00</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>23/07/2016 16:00:00</v>
+        <v>21/07/2016 14:00:00</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" s="4">
         <v>42564.666666666664</v>
       </c>
@@ -400,10 +407,12 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2"/>
       <c r="C8" s="4">
         <v>42564.666666666664</v>
       </c>
@@ -426,8 +435,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
+      <c r="A9" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="4">
@@ -452,8 +461,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
+      <c r="A10" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4">
@@ -479,7 +488,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4">
@@ -505,7 +514,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="4">
@@ -531,7 +540,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="4">
@@ -557,7 +566,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4">
@@ -583,7 +592,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="4">
@@ -609,7 +618,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="4">
@@ -635,7 +644,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="4">
@@ -661,7 +670,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="4">
@@ -687,7 +696,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="4">

</xml_diff>

<commit_message>
Atualizazao de Roteiros.xlsx e melhoria na formatacao da data do submission server.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Roteiros.xlsx
+++ b/leda-submission-server/conf/Roteiros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Roteiro</t>
   </si>
@@ -76,7 +76,7 @@
     <t>R03-01</t>
   </si>
   <si>
-    <t>Ordenacao linear</t>
+    <t>Ordenacao linear - Counting sort</t>
   </si>
   <si>
     <t>Raiff Ramalho de Mello</t>
@@ -88,7 +88,10 @@
     <t>R04-01</t>
   </si>
   <si>
-    <t>Roteiro especial sobre algoritmos de ordenacao</t>
+    <t>Roteiro extra de ordenacao - comb e gnome</t>
+  </si>
+  <si>
+    <t>David de Medeiros Souza</t>
   </si>
   <si>
     <t>R04-02</t>
@@ -97,10 +100,22 @@
     <t>R05-01</t>
   </si>
   <si>
+    <t>Tipo Abstrato de Dado. Vetor, Pilha e Fila</t>
+  </si>
+  <si>
+    <t>César Ferreira Tavares Neto</t>
+  </si>
+  <si>
     <t>R05-02</t>
   </si>
   <si>
     <t>R06-01</t>
+  </si>
+  <si>
+    <t>Lista encadeada (abordagem iterativa)</t>
+  </si>
+  <si>
+    <t>Adson César da Silva</t>
   </si>
   <si>
     <t>R06-02</t>
@@ -226,7 +241,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -500,7 +515,9 @@
         <f t="shared" si="2"/>
         <v>22/07/2016 16:00:00</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>23/07/2016 16:00:00</v>
@@ -512,7 +529,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>25</v>
@@ -528,7 +545,9 @@
         <f t="shared" si="2"/>
         <v>22/07/2016 16:00:00</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>23/07/2016 16:00:00</v>
@@ -540,9 +559,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C11" s="6">
         <v>42583.583333333336</v>
       </c>
@@ -554,7 +575,9 @@
         <f t="shared" si="2"/>
         <v>03/08/2016 14:00:00</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="3"/>
         <v>04/08/2016 14:00:00</v>
@@ -566,9 +589,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C12" s="6">
         <v>42583.583333333336</v>
       </c>
@@ -580,7 +605,9 @@
         <f t="shared" si="2"/>
         <v>03/08/2016 14:00:00</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>04/08/2016 14:00:00</v>
@@ -592,9 +619,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C13" s="6">
         <v>42585.666666666664</v>
       </c>
@@ -606,7 +635,9 @@
         <f t="shared" si="2"/>
         <v>05/08/2016 16:00:00</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>06/08/2016 16:00:00</v>
@@ -618,9 +649,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C14" s="6">
         <v>42585.666666666664</v>
       </c>
@@ -632,7 +665,9 @@
         <f t="shared" si="2"/>
         <v>05/08/2016 16:00:00</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>06/08/2016 16:00:00</v>
@@ -644,7 +679,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="3">
@@ -670,7 +705,7 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="3">
@@ -696,7 +731,7 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="3">
@@ -722,7 +757,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="3">
@@ -748,7 +783,7 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="3">

</xml_diff>

<commit_message>
Mudancas no sender e server para aceitar upload de provas do professor.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Roteiros.xlsx
+++ b/leda-submission-server/conf/Roteiros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Roteiro</t>
   </si>
@@ -100,7 +100,7 @@
     <t>R05-01</t>
   </si>
   <si>
-    <t>Tipo Abstrato de Dado. Vetor, Pilha e Fila</t>
+    <t>Roteiro extra: algoritmo de ordenação</t>
   </si>
   <si>
     <t>César Ferreira Tavares Neto</t>
@@ -112,7 +112,7 @@
     <t>R06-01</t>
   </si>
   <si>
-    <t>Lista encadeada (abordagem iterativa)</t>
+    <t>Tipo Abstrato de Dado. Vetor, Pilha e Fila</t>
   </si>
   <si>
     <t>Adson César da Silva</t>
@@ -121,10 +121,13 @@
     <t>R06-02</t>
   </si>
   <si>
-    <t>R13</t>
+    <t>R07-01</t>
   </si>
   <si>
-    <t>R14</t>
+    <t>Lista encadeada (abordagem iterativa)</t>
+  </si>
+  <si>
+    <t>R07-02</t>
   </si>
   <si>
     <t>R15</t>
@@ -678,10 +681,12 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C15" s="3">
         <v>42564.6666666667</v>
       </c>
@@ -704,10 +709,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4"/>
       <c r="C16" s="3">
         <v>42564.6666666667</v>
       </c>
@@ -731,7 +738,7 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="3">
@@ -757,7 +764,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="3">
@@ -783,7 +790,7 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="3">

</xml_diff>

<commit_message>
Atualizado dados dos roteiros.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Roteiros.xlsx
+++ b/leda-submission-server/conf/Roteiros.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Roteiro</t>
   </si>
@@ -100,13 +100,16 @@
     <t>R05-01</t>
   </si>
   <si>
-    <t>Roteiro extra: algoritmo de ordenação</t>
+    <t>Roteiro extra: algoritmo de ordenação - Odd Even Bubble</t>
   </si>
   <si>
     <t>César Ferreira Tavares Neto</t>
   </si>
   <si>
     <t>R05-02</t>
+  </si>
+  <si>
+    <t>Roteiro extra: algoritmo de ordenação - Odd Even Selection</t>
   </si>
   <si>
     <t>R06-01</t>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>Lista encadeada (abordagem iterativa)</t>
+  </si>
+  <si>
+    <t>Eri Jonhson Oliveira da Silva</t>
   </si>
   <si>
     <t>R07-02</t>
@@ -568,26 +574,26 @@
         <v>29</v>
       </c>
       <c r="C11" s="6">
-        <v>42583.583333333336</v>
+        <v>42607.583333333336</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>02/08/2016 02:00:00</v>
+        <v>26/08/2016 02:00:00</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>03/08/2016 14:00:00</v>
+        <v>27/08/2016 14:00:00</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>04/08/2016 14:00:00</v>
+        <v>28/08/2016 14:00:00</v>
       </c>
       <c r="H11" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>11/08/2016 14:00:00</v>
+        <v>04/09/2016 14:00:00</v>
       </c>
     </row>
     <row r="12">
@@ -595,150 +601,154 @@
         <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6">
-        <v>42583.583333333336</v>
+        <v>42607.583333333336</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>02/08/2016 02:00:00</v>
+        <v>26/08/2016 02:00:00</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>03/08/2016 14:00:00</v>
+        <v>27/08/2016 14:00:00</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>04/08/2016 14:00:00</v>
+        <v>28/08/2016 14:00:00</v>
       </c>
       <c r="H12" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>11/08/2016 14:00:00</v>
+        <v>04/09/2016 14:00:00</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6">
-        <v>42585.666666666664</v>
+        <v>42583.583333333336</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>04/08/2016 04:00:00</v>
+        <v>02/08/2016 02:00:00</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>05/08/2016 16:00:00</v>
+        <v>03/08/2016 14:00:00</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>06/08/2016 16:00:00</v>
+        <v>04/08/2016 14:00:00</v>
       </c>
       <c r="H13" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>13/08/2016 16:00:00</v>
+        <v>11/08/2016 14:00:00</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6">
-        <v>42585.666666666664</v>
+        <v>42583.583333333336</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>04/08/2016 04:00:00</v>
+        <v>02/08/2016 02:00:00</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>05/08/2016 16:00:00</v>
+        <v>03/08/2016 14:00:00</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>06/08/2016 16:00:00</v>
+        <v>04/08/2016 14:00:00</v>
       </c>
       <c r="H14" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>13/08/2016 16:00:00</v>
+        <v>11/08/2016 14:00:00</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="3">
-        <v>42564.6666666667</v>
+        <v>38</v>
+      </c>
+      <c r="C15" s="6">
+        <v>42585.666666666664</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>14/07/2016 04:00:00</v>
+        <v>04/08/2016 04:00:00</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15/07/2016 16:00:00</v>
-      </c>
-      <c r="F15" s="4"/>
+        <v>05/08/2016 16:00:00</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>16/07/2016 16:00:00</v>
+        <v>06/08/2016 16:00:00</v>
       </c>
       <c r="H15" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>23/07/2016 16:00:00</v>
+        <v>13/08/2016 16:00:00</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3">
-        <v>42564.6666666667</v>
+      <c r="C16" s="6">
+        <v>42585.666666666664</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>14/07/2016 04:00:00</v>
+        <v>04/08/2016 04:00:00</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15/07/2016 16:00:00</v>
-      </c>
-      <c r="F16" s="4"/>
+        <v>05/08/2016 16:00:00</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>16/07/2016 16:00:00</v>
+        <v>06/08/2016 16:00:00</v>
       </c>
       <c r="H16" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>23/07/2016 16:00:00</v>
+        <v>13/08/2016 16:00:00</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="3">
@@ -764,7 +774,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="3">
@@ -790,7 +800,7 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="3">

</xml_diff>